<commit_message>
udpate right click menu pop up and edit when click on values
</commit_message>
<xml_diff>
--- a/upload/cringe.xlsx
+++ b/upload/cringe.xlsx
@@ -10,7 +10,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assignments" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$H$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Assignments'!$A$1:$F$5</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -419,7 +419,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -434,8 +434,6 @@
     <col width="13" customWidth="1" min="4" max="4"/>
     <col width="14" customWidth="1" min="5" max="5"/>
     <col width="14" customWidth="1" min="6" max="6"/>
-    <col width="34" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -469,53 +467,13 @@
           <t>publish_time</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>move_folder</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>monetization</t>
-        </is>
-      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>E:\storage\902 - Copy (24).mp4</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>áda</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>11/06/2025</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>E:\ghep xong\902 - Copy (24).mp4</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="5"/>
   </sheetData>
-  <autoFilter ref="A1:H2"/>
+  <autoFilter ref="A1:F5"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>